<commit_message>
update euro2024 matches file
</commit_message>
<xml_diff>
--- a/data/source/competitions/euro2024.xlsx
+++ b/data/source/competitions/euro2024.xlsx
@@ -162,7 +162,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +173,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -204,33 +210,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
@@ -545,8 +554,8 @@
     <col min="2" max="2" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="9" width="18.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="9" width="18.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -566,10 +575,10 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -585,11 +594,11 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="4">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="6">
         <v>45457</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -598,10 +607,10 @@
       <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="1">
         <v>5</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="1">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -617,11 +626,11 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="4">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="5">
         <v>3</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="6">
         <v>45458</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -630,8 +639,12 @@
       <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>3</v>
+      </c>
       <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
@@ -645,11 +658,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="4">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="5">
         <v>4</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="6">
         <v>45458</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -658,8 +671,12 @@
       <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>2</v>
+      </c>
       <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
@@ -673,11 +690,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="4">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="6">
         <v>45458</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -686,8 +703,12 @@
       <c r="D5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>3</v>
+      </c>
       <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
@@ -701,11 +722,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="4">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="5">
         <v>6</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="6">
         <v>45459</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -714,8 +735,8 @@
       <c r="D6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="3" t="s">
         <v>12</v>
       </c>
@@ -729,11 +750,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="4">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="6">
         <v>45459</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -742,8 +763,8 @@
       <c r="D7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="3" t="s">
         <v>12</v>
       </c>
@@ -757,11 +778,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="4">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="6">
         <v>45459</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -770,8 +791,8 @@
       <c r="D8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="3" t="s">
         <v>12</v>
       </c>
@@ -785,11 +806,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="4">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="6">
         <v>45460</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -798,8 +819,8 @@
       <c r="D9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
       <c r="G9" s="3" t="s">
         <v>12</v>
       </c>
@@ -813,11 +834,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="4">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="6">
         <v>45460</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -826,8 +847,8 @@
       <c r="D10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="3" t="s">
         <v>12</v>
       </c>
@@ -841,11 +862,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
         <v>45460</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -854,8 +875,8 @@
       <c r="D11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
       <c r="G11" s="3" t="s">
         <v>12</v>
       </c>
@@ -869,11 +890,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="4">
-        <v>12</v>
-      </c>
-      <c r="B12" s="5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="5">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6">
         <v>45461</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -882,8 +903,8 @@
       <c r="D12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="3" t="s">
         <v>12</v>
       </c>
@@ -897,11 +918,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="4">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="6">
         <v>45461</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -910,8 +931,8 @@
       <c r="D13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="3" t="s">
         <v>12</v>
       </c>
@@ -925,11 +946,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="4">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="6">
         <v>45462</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -938,8 +959,8 @@
       <c r="D14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="3" t="s">
         <v>12</v>
       </c>
@@ -953,11 +974,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="4">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="5">
         <v>15</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="6">
         <v>45462</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -966,8 +987,8 @@
       <c r="D15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="3" t="s">
         <v>12</v>
       </c>
@@ -981,11 +1002,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="4">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="6">
         <v>45462</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -994,8 +1015,8 @@
       <c r="D16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="3" t="s">
         <v>12</v>
       </c>
@@ -1009,11 +1030,11 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="4">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="5">
         <v>17</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="6">
         <v>45463</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1022,8 +1043,8 @@
       <c r="D17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="3" t="s">
         <v>12</v>
       </c>
@@ -1037,11 +1058,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="4">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="6">
         <v>45463</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -1050,8 +1071,8 @@
       <c r="D18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
       <c r="G18" s="3" t="s">
         <v>12</v>
       </c>
@@ -1065,11 +1086,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="B19" s="5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6">
         <v>45463</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1078,8 +1099,8 @@
       <c r="D19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="3" t="s">
         <v>12</v>
       </c>
@@ -1093,11 +1114,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="4">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="5">
         <v>20</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="6">
         <v>45464</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1106,8 +1127,8 @@
       <c r="D20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
       <c r="G20" s="3" t="s">
         <v>12</v>
       </c>
@@ -1121,11 +1142,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="4">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="5">
         <v>19</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="6">
         <v>45464</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1134,8 +1155,8 @@
       <c r="D21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
       <c r="G21" s="3" t="s">
         <v>12</v>
       </c>
@@ -1149,11 +1170,11 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="4">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="6">
         <v>45464</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1162,8 +1183,8 @@
       <c r="D22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
       <c r="G22" s="3" t="s">
         <v>12</v>
       </c>
@@ -1178,10 +1199,10 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="4">
+      <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="6">
         <v>45465</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1190,8 +1211,8 @@
       <c r="D23" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
       <c r="G23" s="3" t="s">
         <v>12</v>
       </c>
@@ -1206,10 +1227,10 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="4">
+      <c r="A24" s="5">
         <v>24</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="6">
         <v>45465</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1218,8 +1239,8 @@
       <c r="D24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
       <c r="G24" s="3" t="s">
         <v>12</v>
       </c>
@@ -1234,10 +1255,10 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="4">
+      <c r="A25" s="5">
         <v>23</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="6">
         <v>45465</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -1246,8 +1267,8 @@
       <c r="D25" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
       <c r="G25" s="3" t="s">
         <v>12</v>
       </c>
@@ -1262,10 +1283,10 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="4">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="6">
         <v>45466</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -1274,8 +1295,8 @@
       <c r="D26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
       <c r="G26" s="3" t="s">
         <v>12</v>
       </c>
@@ -1290,10 +1311,10 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="4">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="6">
         <v>45466</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -1302,8 +1323,8 @@
       <c r="D27" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
       <c r="G27" s="3" t="s">
         <v>12</v>
       </c>
@@ -1318,10 +1339,10 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="4">
+      <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="6">
         <v>45467</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1330,8 +1351,8 @@
       <c r="D28" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
       <c r="G28" s="3" t="s">
         <v>12</v>
       </c>
@@ -1346,10 +1367,10 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="4">
+      <c r="A29" s="5">
         <v>28</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="6">
         <v>45467</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -1358,8 +1379,8 @@
       <c r="D29" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
       <c r="G29" s="3" t="s">
         <v>12</v>
       </c>
@@ -1374,10 +1395,10 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="4">
+      <c r="A30" s="5">
         <v>31</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="6">
         <v>45468</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -1386,8 +1407,8 @@
       <c r="D30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
       <c r="G30" s="3" t="s">
         <v>12</v>
       </c>
@@ -1402,10 +1423,10 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="4">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="6">
         <v>45468</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -1414,8 +1435,8 @@
       <c r="D31" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
       <c r="G31" s="3" t="s">
         <v>12</v>
       </c>
@@ -1430,10 +1451,10 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="4">
+      <c r="A32" s="5">
         <v>29</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="6">
         <v>45468</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -1442,8 +1463,8 @@
       <c r="D32" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
       <c r="G32" s="3" t="s">
         <v>12</v>
       </c>
@@ -1458,10 +1479,10 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="4">
+      <c r="A33" s="5">
         <v>32</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="6">
         <v>45468</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1470,8 +1491,8 @@
       <c r="D33" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
       <c r="G33" s="3" t="s">
         <v>12</v>
       </c>
@@ -1486,10 +1507,10 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="4">
+      <c r="A34" s="5">
         <v>33</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="6">
         <v>45469</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -1498,8 +1519,8 @@
       <c r="D34" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
       <c r="G34" s="3" t="s">
         <v>12</v>
       </c>
@@ -1514,10 +1535,10 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="4">
+      <c r="A35" s="5">
         <v>36</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="6">
         <v>45469</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -1526,8 +1547,8 @@
       <c r="D35" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
       <c r="G35" s="3" t="s">
         <v>12</v>
       </c>
@@ -1542,10 +1563,10 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="4">
+      <c r="A36" s="5">
         <v>34</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="6">
         <v>45469</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -1554,8 +1575,8 @@
       <c r="D36" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
       <c r="G36" s="3" t="s">
         <v>12</v>
       </c>
@@ -1570,10 +1591,10 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="4">
+      <c r="A37" s="5">
         <v>35</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="6">
         <v>45469</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -1582,8 +1603,8 @@
       <c r="D37" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
       <c r="G37" s="3" t="s">
         <v>12</v>
       </c>
@@ -1598,16 +1619,16 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="4">
+      <c r="A38" s="5">
         <v>37</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="6">
         <v>45472</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
       <c r="G38" s="3" t="s">
         <v>12</v>
       </c>
@@ -1620,16 +1641,16 @@
       <c r="J38" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="4">
+      <c r="A39" s="5">
         <v>38</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="6">
         <v>45472</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
       <c r="G39" s="3" t="s">
         <v>12</v>
       </c>
@@ -1642,16 +1663,16 @@
       <c r="J39" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="4">
+      <c r="A40" s="5">
         <v>39</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="6">
         <v>45473</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
       <c r="G40" s="3" t="s">
         <v>12</v>
       </c>
@@ -1664,16 +1685,16 @@
       <c r="J40" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="4">
+      <c r="A41" s="5">
         <v>40</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B41" s="6">
         <v>45473</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
       <c r="G41" s="3" t="s">
         <v>12</v>
       </c>
@@ -1686,16 +1707,16 @@
       <c r="J41" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="4">
+      <c r="A42" s="5">
         <v>41</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="6">
         <v>45474</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
       <c r="G42" s="3" t="s">
         <v>12</v>
       </c>
@@ -1708,16 +1729,16 @@
       <c r="J42" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="4">
+      <c r="A43" s="5">
         <v>42</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B43" s="6">
         <v>45474</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
       <c r="G43" s="3" t="s">
         <v>12</v>
       </c>
@@ -1730,16 +1751,16 @@
       <c r="J43" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="4">
+      <c r="A44" s="5">
         <v>43</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="6">
         <v>45475</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
       <c r="G44" s="3" t="s">
         <v>12</v>
       </c>
@@ -1752,16 +1773,16 @@
       <c r="J44" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="4">
+      <c r="A45" s="5">
         <v>44</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B45" s="6">
         <v>45475</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
       <c r="G45" s="3" t="s">
         <v>12</v>
       </c>
@@ -1774,16 +1795,16 @@
       <c r="J45" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="4">
+      <c r="A46" s="5">
         <v>45</v>
       </c>
-      <c r="B46" s="5">
+      <c r="B46" s="6">
         <v>45478</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
       <c r="G46" s="3" t="s">
         <v>12</v>
       </c>
@@ -1796,16 +1817,16 @@
       <c r="J46" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
-      <c r="A47" s="4">
+      <c r="A47" s="5">
         <v>46</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="6">
         <v>45478</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
       <c r="G47" s="3" t="s">
         <v>12</v>
       </c>
@@ -1818,16 +1839,16 @@
       <c r="J47" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
-      <c r="A48" s="4">
+      <c r="A48" s="5">
         <v>47</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48" s="6">
         <v>45479</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
       <c r="G48" s="3" t="s">
         <v>12</v>
       </c>
@@ -1840,16 +1861,16 @@
       <c r="J48" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
-      <c r="A49" s="4">
+      <c r="A49" s="5">
         <v>48</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B49" s="6">
         <v>45479</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
       <c r="G49" s="3" t="s">
         <v>12</v>
       </c>
@@ -1862,16 +1883,16 @@
       <c r="J49" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
-      <c r="A50" s="4">
+      <c r="A50" s="5">
         <v>49</v>
       </c>
-      <c r="B50" s="5">
+      <c r="B50" s="6">
         <v>45482</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
       <c r="G50" s="3" t="s">
         <v>12</v>
       </c>
@@ -1884,16 +1905,16 @@
       <c r="J50" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
-      <c r="A51" s="4">
+      <c r="A51" s="5">
         <v>50</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51" s="6">
         <v>45483</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
       <c r="G51" s="3" t="s">
         <v>12</v>
       </c>
@@ -1906,16 +1927,16 @@
       <c r="J51" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
-      <c r="A52" s="4">
+      <c r="A52" s="5">
         <v>51</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="6">
         <v>45487</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
       <c r="G52" s="3" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
euro 2024 match update and countries color codes
</commit_message>
<xml_diff>
--- a/data/source/competitions/euro2024.xlsx
+++ b/data/source/competitions/euro2024.xlsx
@@ -912,8 +912,12 @@
       <c r="D12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
       <c r="G12" s="3" t="s">
         <v>12</v>
       </c>
@@ -940,8 +944,12 @@
       <c r="D13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3</v>
+      </c>
       <c r="G13" s="3" t="s">
         <v>12</v>
       </c>

</xml_diff>